<commit_message>
Laboratorio 7 - Doc Pruebas - Est 1
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/2022-20/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana Sofía Rozo C\Documents\Repositorios estructuras de datos y algoritmos\LabCollision-S08-G01\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="726" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F54888-DFB5-49D6-8E23-12D138256747}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA7183B-99B4-4E9E-9C8D-1E8DEF597D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="887" windowWidth="2273" windowHeight="1493" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="767" activeTab="2" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -193,9 +193,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -208,37 +205,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -391,6 +368,32 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -459,7 +462,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -532,7 +535,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -619,7 +622,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -630,17 +633,17 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>34929.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>34929.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>34929.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>35114.089999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,16 +655,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>251.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>225.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>194.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>189.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -750,7 +753,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -762,13 +765,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>35114.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>35114.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35282.559999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>45348.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,13 +786,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>214.91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>203.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>203.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>206.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -881,11 +890,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -919,7 +928,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1087681551"/>
@@ -1006,7 +1015,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1044,7 +1053,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1087686127"/>
@@ -1086,7 +1095,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1116,7 +1125,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1125,7 +1134,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1189,7 +1198,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1313,7 +1322,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1345,17 +1354,17 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>34929.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>34929.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>34929.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>35114.089999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,7 +1480,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1504,13 +1513,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>35114.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>35114.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35282.559999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>45348.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,7 +1612,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1635,7 +1647,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1086959919"/>
@@ -1708,11 +1720,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1742,7 +1754,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1086958255"/>
@@ -1781,7 +1793,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1811,7 +1823,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2890,7 +2902,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CAFD5B44-21B9-42C7-B503-C146EF1BA3EE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2901,7 +2913,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{680E7371-595A-4F03-ABE3-E0257A96E5F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2912,7 +2924,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8659091" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2945,7 +2957,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8659091" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2980,26 +2992,26 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
     <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3297,25 +3309,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
-    <row r="2" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3326,64 +3338,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="10">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>0.1</v>
       </c>
-      <c r="B3" s="5">
-        <v>100</v>
+      <c r="B3" s="14">
+        <v>34929.78</v>
       </c>
       <c r="C3" s="8">
-        <v>75</v>
+        <v>251.05</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="11">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>0.5</v>
       </c>
       <c r="B4" s="6">
-        <f>B3+40</f>
-        <v>140</v>
+        <v>34929.78</v>
       </c>
       <c r="C4" s="8">
-        <f>C3+10</f>
-        <v>85</v>
+        <v>225.16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="10">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <v>0.7</v>
       </c>
       <c r="B5" s="6">
-        <f>B4+40</f>
-        <v>180</v>
+        <v>34929.78</v>
       </c>
       <c r="C5" s="8">
-        <f>C4+10</f>
-        <v>95</v>
+        <v>194.11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
         <v>0.9</v>
       </c>
       <c r="B6" s="6">
-        <f>B5+40</f>
-        <v>220</v>
+        <v>35114.089999999997</v>
       </c>
       <c r="C6" s="8">
-        <f>C5+10</f>
-        <v>105</v>
+        <v>189.27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.5">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -3394,51 +3400,51 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" s="2">
-        <v>100</v>
+        <v>35114.82</v>
       </c>
       <c r="C11" s="5">
-        <v>105</v>
+        <v>214.91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2">
-        <f>B11+30</f>
-        <v>130</v>
+        <v>35114.82</v>
       </c>
       <c r="C12" s="6">
-        <f>C11+20</f>
-        <v>125</v>
+        <v>203.05</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="12">
+        <v>35282.559999999998</v>
+      </c>
+      <c r="C13" s="12">
+        <v>203.16</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>8</v>
       </c>
       <c r="B14" s="2">
-        <f>B12+30</f>
-        <v>160</v>
+        <v>45348.3</v>
       </c>
       <c r="C14" s="6">
-        <f>C12+20</f>
-        <v>145</v>
+        <v>206.98</v>
       </c>
     </row>
-    <row r="23" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="23" ht="14.7" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -3453,6 +3459,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a4df9e4b793c0fa050084ef4feafa589">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="067b7080d2289f9ba15465beea7d18a8" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -3689,27 +3715,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF363B8-2236-4100-84F9-92CAF618B773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3726,29 +3757,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>